<commit_message>
Revert "Revert "eliminar firmadas""
This reverts commit 1c0ef4b99eff80db4f5ad88df286b921f9fe0f4c.
</commit_message>
<xml_diff>
--- a/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relación 4 oral pendientes de subir al sistema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Respaldo en Computadora" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Formato entrega " sheetId="5" r:id="rId4"/>
     <sheet name="Quemados" sheetId="2" r:id="rId5"/>
     <sheet name="conteo audiencias" sheetId="6" r:id="rId6"/>
-    <sheet name="firmadas fuera de tiempo" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="143">
   <si>
     <t>Expediente</t>
   </si>
@@ -459,150 +458,6 @@
   </si>
   <si>
     <t>582 GB</t>
-  </si>
-  <si>
-    <t>dia agenda</t>
-  </si>
-  <si>
-    <t>descripción</t>
-  </si>
-  <si>
-    <t>cantidad de archivos</t>
-  </si>
-  <si>
-    <t>fecha firma</t>
-  </si>
-  <si>
-    <t>162/2017</t>
-  </si>
-  <si>
-    <t>298/2018</t>
-  </si>
-  <si>
-    <t>1683/2017</t>
-  </si>
-  <si>
-    <t>91/2018</t>
-  </si>
-  <si>
-    <t>1023/2017</t>
-  </si>
-  <si>
-    <t>1425/2017</t>
-  </si>
-  <si>
-    <t>20/2018</t>
-  </si>
-  <si>
-    <t>1152/2017</t>
-  </si>
-  <si>
-    <t>210/2018</t>
-  </si>
-  <si>
-    <t>18/2017</t>
-  </si>
-  <si>
-    <t>834/2017</t>
-  </si>
-  <si>
-    <t>no esta agendado</t>
-  </si>
-  <si>
-    <t>1404/2017</t>
-  </si>
-  <si>
-    <t>1281/2017</t>
-  </si>
-  <si>
-    <t>1597/2017</t>
-  </si>
-  <si>
-    <t>167/2018</t>
-  </si>
-  <si>
-    <t>169/2018</t>
-  </si>
-  <si>
-    <t>886/2017</t>
-  </si>
-  <si>
-    <t>442/2017</t>
-  </si>
-  <si>
-    <t>794/2017</t>
-  </si>
-  <si>
-    <t>247/2017</t>
-  </si>
-  <si>
-    <t>67/2018</t>
-  </si>
-  <si>
-    <t>133/2016</t>
-  </si>
-  <si>
-    <t>1647/2017</t>
-  </si>
-  <si>
-    <t>197/2017</t>
-  </si>
-  <si>
-    <t>164/2018</t>
-  </si>
-  <si>
-    <t>1608/2017</t>
-  </si>
-  <si>
-    <t>168/2016</t>
-  </si>
-  <si>
-    <t>493/2017</t>
-  </si>
-  <si>
-    <t>267/2017</t>
-  </si>
-  <si>
-    <t>183/2018</t>
-  </si>
-  <si>
-    <t>891/2017</t>
-  </si>
-  <si>
-    <t>1549/2017</t>
-  </si>
-  <si>
-    <t>168/2018</t>
-  </si>
-  <si>
-    <t>254/2018</t>
-  </si>
-  <si>
-    <t>146/2018</t>
-  </si>
-  <si>
-    <t>1576/2017</t>
-  </si>
-  <si>
-    <t>1330/2017</t>
-  </si>
-  <si>
-    <t>145/2018</t>
-  </si>
-  <si>
-    <t>1501/2017</t>
-  </si>
-  <si>
-    <t>171/2018</t>
-  </si>
-  <si>
-    <t>763/2017</t>
-  </si>
-  <si>
-    <t>323/2017</t>
-  </si>
-  <si>
-    <t>63/2018</t>
   </si>
 </sst>
 </file>
@@ -967,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2953,7 +2808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -3081,1104 +2936,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43265</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43265</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43265</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43265</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43265</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43264</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43263</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43263</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1">
-        <v>43263</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="1">
-        <v>43263</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="1">
-        <v>43258</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="1">
-        <v>43258</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1">
-        <v>43258</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="1">
-        <v>43258</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="1">
-        <v>43258</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="1">
-        <v>43258</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1">
-        <v>43257</v>
-      </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1">
-        <v>43256</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="1">
-        <v>43256</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="1">
-        <v>43256</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="1">
-        <v>43256</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B23" s="1">
-        <v>43223</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="1">
-        <v>43223</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B25" s="1">
-        <v>43223</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="1">
-        <v>43223</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B27" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B28" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B29" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B30" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B31" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B32" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="1">
-        <v>43228</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B34" s="1">
-        <v>43229</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="1">
-        <v>43229</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B36" s="1">
-        <v>43229</v>
-      </c>
-      <c r="C36" s="2">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B37" s="1">
-        <v>43229</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="1">
-        <v>43229</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="1">
-        <v>43235</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="1">
-        <v>43235</v>
-      </c>
-      <c r="C40" s="2">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="1">
-        <v>43235</v>
-      </c>
-      <c r="C41" s="2">
-        <v>2</v>
-      </c>
-      <c r="D41" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B42" s="1">
-        <v>43235</v>
-      </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B43" s="1">
-        <v>43235</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="1">
-        <v>43237</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B45" s="1">
-        <v>43237</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B46" s="1">
-        <v>43237</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B47" s="1">
-        <v>43237</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B48" s="1">
-        <v>43237</v>
-      </c>
-      <c r="C48" s="2">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B49" s="1">
-        <v>43242</v>
-      </c>
-      <c r="C49" s="2">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B50" s="1">
-        <v>43242</v>
-      </c>
-      <c r="C50" s="2">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="1">
-        <v>43242</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B52" s="1">
-        <v>43242</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B53" s="1">
-        <v>43242</v>
-      </c>
-      <c r="C53" s="2">
-        <v>1</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="1">
-        <v>43242</v>
-      </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="1">
-        <v>43244</v>
-      </c>
-      <c r="C55" s="2">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B56" s="1">
-        <v>43244</v>
-      </c>
-      <c r="C56" s="2">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B57" s="1">
-        <v>43244</v>
-      </c>
-      <c r="C57" s="2">
-        <v>1</v>
-      </c>
-      <c r="D57" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B58" s="1">
-        <v>43244</v>
-      </c>
-      <c r="C58" s="2">
-        <v>1</v>
-      </c>
-      <c r="D58" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B59" s="1">
-        <v>43244</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
-      <c r="D59" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" s="1">
-        <v>43244</v>
-      </c>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-      <c r="D60" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B61" s="1">
-        <v>43249</v>
-      </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B62" s="1">
-        <v>43249</v>
-      </c>
-      <c r="C62" s="2">
-        <v>1</v>
-      </c>
-      <c r="D62" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B63" s="1">
-        <v>43249</v>
-      </c>
-      <c r="C63" s="2">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B64" s="1">
-        <v>43249</v>
-      </c>
-      <c r="C64" s="2">
-        <v>2</v>
-      </c>
-      <c r="D64" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="1">
-        <v>43249</v>
-      </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B66" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C66" s="2">
-        <v>1</v>
-      </c>
-      <c r="D66" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B67" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-      <c r="D67" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B68" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C68" s="2">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B69" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C69" s="2">
-        <v>1</v>
-      </c>
-      <c r="D69" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B70" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
-      <c r="D70" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B71" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C71" s="2">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B72" s="1">
-        <v>43251</v>
-      </c>
-      <c r="C72" s="2">
-        <v>1</v>
-      </c>
-      <c r="D72" s="1">
-        <v>43325</v>
-      </c>
-      <c r="E72" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
actualize respaldo en dd
actualize la cantidad de audiencias respaldadas en el disco duro del juzgado
</commit_message>
<xml_diff>
--- a/relación 4 oral pendientes de subir al sistema.xlsx
+++ b/relación 4 oral pendientes de subir al sistema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="4920" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Respaldo en Computadora" sheetId="1" r:id="rId1"/>
@@ -443,12 +443,6 @@
     <t>3 ARCHIVOS</t>
   </si>
   <si>
-    <t>330 GB</t>
-  </si>
-  <si>
-    <t>567 GB</t>
-  </si>
-  <si>
     <t>328 GB</t>
   </si>
   <si>
@@ -789,6 +783,12 @@
   </si>
   <si>
     <t>11/2018</t>
+  </si>
+  <si>
+    <t>337 GB</t>
+  </si>
+  <si>
+    <t>560 GB</t>
   </si>
 </sst>
 </file>
@@ -2393,8 +2393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2480,19 +2480,19 @@
         <v>115</v>
       </c>
       <c r="B4">
-        <v>855</v>
+        <v>878</v>
       </c>
       <c r="C4">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
       <c r="F4" s="1">
-        <v>43322</v>
+        <v>43335</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -2506,10 +2506,10 @@
         <v>230</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F5" s="1">
         <v>43322</v>
@@ -3252,16 +3252,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="D1" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -3536,7 +3536,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B20" s="13">
         <v>43256</v>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B21" s="13">
         <v>43256</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B23" s="13">
         <v>43223</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B24" s="13">
         <v>43223</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B25" s="13">
         <v>43223</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" s="13">
         <v>43223</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B27" s="13">
         <v>43228</v>
@@ -3656,7 +3656,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B28" s="13">
         <v>43228</v>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B29" s="13">
         <v>43228</v>
@@ -3686,7 +3686,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B30" s="13">
         <v>43228</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B31" s="13">
         <v>43228</v>
@@ -3711,12 +3711,12 @@
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B32" s="13">
         <v>43228</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B34" s="13">
         <v>43229</v>
@@ -3761,7 +3761,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B35" s="13">
         <v>43229</v>
@@ -3776,7 +3776,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B36" s="13">
         <v>43229</v>
@@ -3791,7 +3791,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B37" s="13">
         <v>43229</v>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B41" s="13">
         <v>43235</v>
@@ -3866,7 +3866,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B42" s="13">
         <v>43235</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B43" s="13">
         <v>43235</v>
@@ -3896,7 +3896,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B44" s="13">
         <v>43237</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B45" s="13">
         <v>43237</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B46" s="13">
         <v>43237</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B47" s="13">
         <v>43237</v>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B48" s="13">
         <v>43237</v>
@@ -3966,12 +3966,12 @@
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B49" s="13">
         <v>43242</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B50" s="13">
         <v>43242</v>
@@ -4011,12 +4011,12 @@
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B52" s="13">
         <v>43242</v>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -4061,7 +4061,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B55" s="13">
         <v>43244</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B56" s="13">
         <v>43244</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B57" s="13">
         <v>43244</v>
@@ -4106,7 +4106,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B58" s="13">
         <v>43244</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B59" s="13">
         <v>43244</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B60" s="13">
         <v>43244</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B61" s="13">
         <v>43249</v>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B62" s="13">
         <v>43249</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B63" s="13">
         <v>43249</v>
@@ -4196,7 +4196,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B64" s="13">
         <v>43249</v>
@@ -4211,7 +4211,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B65" s="13">
         <v>43249</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B66" s="13">
         <v>43251</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B67" s="13">
         <v>43251</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B68" s="13">
         <v>43251</v>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B69" s="13">
         <v>43251</v>
@@ -4286,7 +4286,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B70" s="13">
         <v>43251</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B71" s="13">
         <v>43251</v>
@@ -4316,7 +4316,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B72" s="13">
         <v>43251</v>
@@ -4331,7 +4331,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B73" s="13">
         <v>43192</v>
@@ -4346,7 +4346,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B74" s="13">
         <v>43193</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B75" s="13">
         <v>43193</v>
@@ -4369,12 +4369,12 @@
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B76" s="13">
         <v>43193</v>
@@ -4389,7 +4389,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B77" s="13">
         <v>43193</v>
@@ -4404,7 +4404,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B78" s="13">
         <v>43193</v>
@@ -4419,7 +4419,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B79" s="13">
         <v>43195</v>
@@ -4434,7 +4434,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B80" s="13">
         <v>43195</v>
@@ -4449,7 +4449,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B81" s="13">
         <v>43195</v>
@@ -4464,7 +4464,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B82" s="13">
         <v>43195</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B83" s="13">
         <v>43200</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B84" s="13">
         <v>43200</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B85" s="13">
         <v>43200</v>
@@ -4524,7 +4524,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B86" s="13">
         <v>43202</v>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B87" s="13">
         <v>43202</v>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B88" s="13">
         <v>43202</v>
@@ -4569,7 +4569,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B89" s="13">
         <v>43202</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B91" s="13">
         <v>43202</v>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B92" s="13">
         <v>43207</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B93" s="13">
         <v>43207</v>
@@ -4644,7 +4644,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B94" s="13">
         <v>43207</v>
@@ -4659,7 +4659,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B95" s="13">
         <v>43207</v>
@@ -4674,7 +4674,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B96" s="13">
         <v>43209</v>
@@ -4682,12 +4682,12 @@
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B97" s="13">
         <v>43209</v>
@@ -4702,7 +4702,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B98" s="13">
         <v>43209</v>
@@ -4717,7 +4717,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B99" s="13">
         <v>43209</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B100" s="13">
         <v>43209</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B101" s="13">
         <v>43209</v>
@@ -4762,7 +4762,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B102" s="13">
         <v>43214</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B103" s="13">
         <v>43214</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B104" s="13">
         <v>43214</v>
@@ -4807,7 +4807,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B105" s="13">
         <v>43214</v>
@@ -4822,7 +4822,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B106" s="13">
         <v>43216</v>
@@ -4830,12 +4830,12 @@
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B107" s="13">
         <v>43216</v>
@@ -4858,12 +4858,12 @@
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B109" s="13">
         <v>43216</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B110" s="13">
         <v>43216</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B111" s="13">
         <v>43216</v>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B112" s="13">
         <v>43216</v>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B113" s="13">
         <v>43160</v>
@@ -4938,7 +4938,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B114" s="13">
         <v>43160</v>
@@ -4953,7 +4953,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B115" s="13">
         <v>43160</v>
@@ -4968,7 +4968,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B116" s="13">
         <v>43160</v>
@@ -4983,7 +4983,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B117" s="13">
         <v>43165</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B118" s="13">
         <v>43165</v>
@@ -5013,7 +5013,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B119" s="13">
         <v>43165</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B120" s="13">
         <v>43165</v>
@@ -5036,12 +5036,12 @@
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B121" s="13">
         <v>43165</v>
@@ -5056,7 +5056,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B122" s="13">
         <v>43165</v>
@@ -5071,7 +5071,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B123" s="13">
         <v>43167</v>
@@ -5086,7 +5086,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B124" s="13">
         <v>43167</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B125" s="13">
         <v>43167</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B126" s="13">
         <v>43167</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B127" s="13">
         <v>43167</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B128" s="13">
         <v>43172</v>
@@ -5154,12 +5154,12 @@
       <c r="C128" s="12"/>
       <c r="D128" s="12"/>
       <c r="E128" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B129" s="13">
         <v>43172</v>
@@ -5174,7 +5174,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B130" s="13">
         <v>43172</v>
@@ -5189,7 +5189,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B131" s="13">
         <v>43172</v>
@@ -5197,12 +5197,12 @@
       <c r="C131" s="12"/>
       <c r="D131" s="12"/>
       <c r="E131" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B132" s="13">
         <v>43172</v>
@@ -5217,7 +5217,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B133" s="13">
         <v>43172</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B134" s="13">
         <v>43174</v>
@@ -5247,7 +5247,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B135" s="13">
         <v>43174</v>
@@ -5262,7 +5262,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B136" s="13">
         <v>43174</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B137" s="13">
         <v>43174</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B138" s="13">
         <v>43174</v>
@@ -5307,7 +5307,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B139" s="13">
         <v>43174</v>
@@ -5315,12 +5315,12 @@
       <c r="C139" s="12"/>
       <c r="D139" s="12"/>
       <c r="E139" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B140" s="13">
         <v>43179</v>
@@ -5335,7 +5335,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B141" s="13">
         <v>43179</v>
@@ -5350,7 +5350,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B142" s="13">
         <v>43179</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B143" s="13">
         <v>43179</v>
@@ -5380,7 +5380,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B144" s="13">
         <v>43179</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B145" s="13">
         <v>43179</v>
@@ -5410,7 +5410,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B146" s="13">
         <v>43181</v>
@@ -5425,7 +5425,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B147" s="13">
         <v>43181</v>
@@ -5440,7 +5440,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B148" s="13">
         <v>43181</v>
@@ -5455,7 +5455,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B149" s="13">
         <v>43181</v>
@@ -5470,7 +5470,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B150" s="13">
         <v>43181</v>
@@ -5493,7 +5493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -5508,21 +5508,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="D1" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B2" s="13">
         <v>43228</v>
@@ -5530,12 +5530,12 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" s="13">
         <v>43237</v>
@@ -5543,7 +5543,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -5556,7 +5556,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -5569,12 +5569,12 @@
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" s="13">
         <v>43193</v>
@@ -5582,12 +5582,12 @@
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B7" s="13">
         <v>43209</v>
@@ -5595,12 +5595,12 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B8" s="13">
         <v>43216</v>
@@ -5608,7 +5608,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -5621,12 +5621,12 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B10" s="13">
         <v>43165</v>
@@ -5634,12 +5634,12 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B11" s="13">
         <v>43172</v>
@@ -5647,12 +5647,12 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B12" s="13">
         <v>43172</v>
@@ -5660,12 +5660,12 @@
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B13" s="13">
         <v>43174</v>
@@ -5673,7 +5673,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>